<commit_message>
Update Codex task backlog spreadsheet
Revised Docs/Codex_Task_Backlog-20251201.xlsx with new or updated task information.
</commit_message>
<xml_diff>
--- a/Docs/Codex_Task_Backlog-20251201.xlsx
+++ b/Docs/Codex_Task_Backlog-20251201.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\LalaLaunchPlugin\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D5ADA1-8F24-4BD9-82D2-1F2B24F1A81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAF4562-8F6F-44CC-82DA-AC1AC5922932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Tasking Order" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasking Order" sheetId="2" r:id="rId1"/>
+    <sheet name="Backlog" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$G$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$G$19</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="151">
   <si>
     <t>ID</t>
   </si>
@@ -563,6 +563,76 @@
   </si>
   <si>
     <t>LALA-022: Add a “Refresh” button to the Fuel Calculator tab that forces a full re-sync of the planner from current truth sources without wiping live-mined data. Place the button alongside the existing “Save All to Profile” control and its modified helper. When clicked, the button should trigger a new public method in FuelCalcs (e.g. RefreshPlannerView) that re-loads profile and track data for the currently selected car/track using the existing LoadProfileData/track-resolution logic, re-applies current session and race context (race length, laps, timer, pit rules), and then re-runs the strategy calculation and updates all UI-bound planner output fields. The refresh must not clear or reset the live fuel model’s sample windows, LiveFuelPerLap, leader pace, or confidence; it should simply recompute derived values and outputs based on the latest profile + live state. If no valid profile/track/session is available, put the planner into a safe “no data” state. The button must not implicitly save any data to disk or change ActiveProfile.</t>
+  </si>
+  <si>
+    <t>Codex Task Completion Summary</t>
+  </si>
+  <si>
+    <t>Tracked the active live car/track combination and treat changes as new live sessions so snapshots reset when either value differs while preserving data across session-type swaps on the same combo.
+Added a comprehensive live snapshot reset that clears lap pace, leader delta, fuel averages, and confidence so new car/track combinations start from profile defaults or empty live data  https://github.com/Lalabot77/LalaLaunchPlugin/pull/137</t>
+  </si>
+  <si>
+    <t>Updated the extra-time-after-zero helper to use a continuous decimal-lap calculation based on leader and driver lap times, ensuring smoother “Est. Drive Time After Timer Zero” updates with pace slider changes.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/139</t>
+  </si>
+  <si>
+    <t>Added leader pace delta tracking with helper updates and resets so SimHub never surfaces stale leader pace data when averages change or telemetry is unavailable.
+Exposed new SimHub parameters for leader average lap time and leader-versus-player delta alongside existing pace metrics.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/140</t>
+  </si>
+  <si>
+    <t>Live max fuel snapshot and helper text now share a common refresh path that always raises property changes and clears to default values when live data is absent, keeping both displays synchronized.
+Added an ApplyLiveMaxFuelSuggestion command and “Set live” button so the max fuel override can adopt the live-detected tank size whenever available.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/138</t>
+  </si>
+  <si>
+    <t>Added telemetry-driven automatic track condition switching with manual override tracking, UI labeling, and reset on session changes so pace and fuel calculations stay aligned with the active state.
+Reset override status when car or track selections change and refreshed initialization to expose the current mode to the UI.
+Added helper text to the Fuel tab to indicate whether the track condition is automatic or manually overridden.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/141</t>
+  </si>
+  <si>
+    <t>Removed the implicit apply from SaveProfiles, so saving profiles now only serializes data and logs without touching the live session; applying remains gated by the explicit command.
+Added planner dirty tracking that flags edits to planner fields, clears when profile data is loaded or saved, and surfaces a “(modified)” hint beside the Save All to Profile button.
+Introduced an exit prompt that offers to persist higher-quality live fuel data back to the active profile before shutdown, wiring it into plugin teardown.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/142</t>
+  </si>
+  <si>
+    <t>Added a Refresh command in the fuel planner to realign the active profile and track selection with live identifiers, reapply planning data, and recompute strategy outputs without clearing live samples.
+Introduced a Refresh button beside “Save All to Profile” on the Fuel tab to trigger the new planner resync flow.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/143</t>
+  </si>
+  <si>
+    <t>Reworked preset application to reuse a shared ApplyPresetValues helper so applied presets stay in sync without replacing list entries. 
+Centralized preset management around _availablePresets with shared helpers for cloning, naming, saving, deleting, and renaming while keeping selected/applied pointers consistent and persisting changes once. 
+Updated the Presets tab actions to rely on the unified FuelCalcs helpers when saving edits, creating defaults, and saving Fuel tab data so selections stay stable across tabs.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/144</t>
+  </si>
+  <si>
+    <t>Added a helper label beside the preset name field to show the Fuel tab’s active preset and highlight when the edited preset matches it.
+Introduced view logic to surface the active preset name, track matches against the local editor selection, and react to Fuel tab changes via property notifications.
+Exposed the applied preset from the fuel calculator and notified bindings when it changes so the Presets tab can reflect the active template status.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/145</t>
+  </si>
+  <si>
+    <t>LALA-39</t>
+  </si>
+  <si>
+    <t>Average Lap Text box not switching between live and profile settings</t>
+  </si>
+  <si>
+    <t>When toggling between Profile and Live data (and when live Avg Lap data available), the text box for Avg Lap should populate Profile or Live value autmatically when Profile and Live toggle is used. There should still be a means to overwrite the data manually until next time the toggle is used. It should also update as the live avg value changes in real time.</t>
+  </si>
+  <si>
+    <t>Toggle between Live and Profile will always load the corresponding Avg Lap value when available.
+Manual overwrite still possible (in profile mode as live would recover each lap crossing)
+Live data should update in textbox when the live avg value is updated.</t>
+  </si>
+  <si>
+    <t>Added weighted fuel and pace confidence calculations that combine seeded versus fresh sample strength, variance checks, wet/dry alignment penalties, and fallback usage so early race confidence stays moderate until new laps arrive.
+Tracked seed presence, fresh sample counts, and fallback flags while resetting models on session transitions to ensure seeded race starts begin with controlled confidence that grows with clean laps.
+Detected car/track changes to clear stored seeds and confidence immediately, preventing stale values from surfacing in the Fuel tab or SimHub outputs.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/146</t>
   </si>
 </sst>
 </file>
@@ -1125,12 +1195,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7016752-5182-4E3D-A00B-D45E03FD7457}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,14 +1228,14 @@
     <col min="5" max="5" width="49.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="61.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="76.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="52.5703125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="19.42578125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="9" width="76.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="52.5703125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="19.42578125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1174,19 +1261,22 @@
         <v>64</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1211,17 +1301,17 @@
       <c r="H2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1246,14 +1336,14 @@
       <c r="H3" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1278,14 +1368,14 @@
       <c r="H4" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="360" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="360" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1305,19 +1395,22 @@
         <v>128</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1342,14 +1435,14 @@
       <c r="H6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1374,11 +1467,11 @@
       <c r="H7" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1403,11 +1496,11 @@
       <c r="H8" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="330" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="330" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1427,13 +1520,16 @@
         <v>134</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="240" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="240" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1453,13 +1549,16 @@
         <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="345" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="345" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1479,13 +1578,16 @@
         <v>103</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1505,13 +1607,16 @@
         <v>102</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="300" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1531,13 +1636,16 @@
         <v>101</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="375" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="375" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1557,13 +1665,16 @@
         <v>87</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="360" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="360" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1589,7 +1700,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="390" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="390" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1614,11 +1725,11 @@
       <c r="H16" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="375" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="375" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1638,13 +1749,16 @@
         <v>111</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1664,13 +1778,16 @@
         <v>115</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="300" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>66</v>
       </c>
@@ -1690,10 +1807,36 @@
         <v>100</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>71</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1701,27 +1844,12 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{D81714E3-95B9-4626-AB5E-00A17ED1FB5D}">
-      <formula1>$K$2:$K$8</formula1>
+      <formula1>$L$2:$L$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{92EF3442-A954-4B29-A8F2-79B2DE268878}">
-      <formula1>$L$2:$L$7</formula1>
+      <formula1>$M$2:$M$7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7016752-5182-4E3D-A00B-D45E03FD7457}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>